<commit_message>
Translated up to ThermoParams
Translated up to ThermoParams. Tough to deal with the CartesianIndices.
</commit_message>
<xml_diff>
--- a/lib/pre-processing/test_file.xlsx
+++ b/lib/pre-processing/test_file.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tsbie\Documents\Universiteit\Master\Jaar 2\MEP\Code\IbM-Fermentation\IbM-Fermentation\lib\pre-processing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{297A48E8-8818-4DD3-9890-B0C58CE260FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{691D60B8-FDC5-49F6-87B5-71A8A05F3C8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14310" yWindow="-16200" windowWidth="14610" windowHeight="15585" tabRatio="808" firstSheet="3" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14310" yWindow="-16200" windowWidth="14610" windowHeight="15585" tabRatio="808" firstSheet="5" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Information" sheetId="30" r:id="rId1"/>
     <sheet name="Reactions" sheetId="18" state="hidden" r:id="rId2"/>
     <sheet name="Settings" sheetId="34" r:id="rId3"/>
-    <sheet name="Discretization" sheetId="27" r:id="rId4"/>
-    <sheet name="Parameters" sheetId="26" r:id="rId5"/>
+    <sheet name="Parameters" sheetId="26" r:id="rId4"/>
+    <sheet name="Discretization" sheetId="27" r:id="rId5"/>
     <sheet name="Diffusion" sheetId="28" r:id="rId6"/>
     <sheet name="Bacteria" sheetId="25" r:id="rId7"/>
     <sheet name="Solver" sheetId="29" r:id="rId8"/>
@@ -30,33 +30,33 @@
     <sheet name="ReactionMatrix" sheetId="21" r:id="rId15"/>
   </sheets>
   <definedNames>
-    <definedName name="solver_adj" localSheetId="4" hidden="1">Parameters!$B$10</definedName>
-    <definedName name="solver_cvg" localSheetId="4" hidden="1">0.0001</definedName>
-    <definedName name="solver_drv" localSheetId="4" hidden="1">1</definedName>
-    <definedName name="solver_eng" localSheetId="4" hidden="1">1</definedName>
-    <definedName name="solver_est" localSheetId="4" hidden="1">1</definedName>
-    <definedName name="solver_itr" localSheetId="4" hidden="1">2147483647</definedName>
-    <definedName name="solver_mip" localSheetId="4" hidden="1">2147483647</definedName>
-    <definedName name="solver_mni" localSheetId="4" hidden="1">30</definedName>
-    <definedName name="solver_mrt" localSheetId="4" hidden="1">0.075</definedName>
-    <definedName name="solver_msl" localSheetId="4" hidden="1">2</definedName>
-    <definedName name="solver_neg" localSheetId="4" hidden="1">1</definedName>
-    <definedName name="solver_nod" localSheetId="4" hidden="1">2147483647</definedName>
-    <definedName name="solver_num" localSheetId="4" hidden="1">0</definedName>
-    <definedName name="solver_nwt" localSheetId="4" hidden="1">1</definedName>
-    <definedName name="solver_opt" localSheetId="4" hidden="1">Parameters!$B$8</definedName>
-    <definedName name="solver_pre" localSheetId="4" hidden="1">0.000001</definedName>
-    <definedName name="solver_rbv" localSheetId="4" hidden="1">1</definedName>
-    <definedName name="solver_rlx" localSheetId="4" hidden="1">2</definedName>
-    <definedName name="solver_rsd" localSheetId="4" hidden="1">0</definedName>
-    <definedName name="solver_scl" localSheetId="4" hidden="1">1</definedName>
-    <definedName name="solver_sho" localSheetId="4" hidden="1">2</definedName>
-    <definedName name="solver_ssz" localSheetId="4" hidden="1">100</definedName>
-    <definedName name="solver_tim" localSheetId="4" hidden="1">2147483647</definedName>
-    <definedName name="solver_tol" localSheetId="4" hidden="1">0.01</definedName>
-    <definedName name="solver_typ" localSheetId="4" hidden="1">3</definedName>
-    <definedName name="solver_val" localSheetId="4" hidden="1">0.000000000135</definedName>
-    <definedName name="solver_ver" localSheetId="4" hidden="1">3</definedName>
+    <definedName name="solver_adj" localSheetId="3" hidden="1">Parameters!$B$10</definedName>
+    <definedName name="solver_cvg" localSheetId="3" hidden="1">0.0001</definedName>
+    <definedName name="solver_drv" localSheetId="3" hidden="1">1</definedName>
+    <definedName name="solver_eng" localSheetId="3" hidden="1">1</definedName>
+    <definedName name="solver_est" localSheetId="3" hidden="1">1</definedName>
+    <definedName name="solver_itr" localSheetId="3" hidden="1">2147483647</definedName>
+    <definedName name="solver_mip" localSheetId="3" hidden="1">2147483647</definedName>
+    <definedName name="solver_mni" localSheetId="3" hidden="1">30</definedName>
+    <definedName name="solver_mrt" localSheetId="3" hidden="1">0.075</definedName>
+    <definedName name="solver_msl" localSheetId="3" hidden="1">2</definedName>
+    <definedName name="solver_neg" localSheetId="3" hidden="1">1</definedName>
+    <definedName name="solver_nod" localSheetId="3" hidden="1">2147483647</definedName>
+    <definedName name="solver_num" localSheetId="3" hidden="1">0</definedName>
+    <definedName name="solver_nwt" localSheetId="3" hidden="1">1</definedName>
+    <definedName name="solver_opt" localSheetId="3" hidden="1">Parameters!$B$8</definedName>
+    <definedName name="solver_pre" localSheetId="3" hidden="1">0.000001</definedName>
+    <definedName name="solver_rbv" localSheetId="3" hidden="1">1</definedName>
+    <definedName name="solver_rlx" localSheetId="3" hidden="1">2</definedName>
+    <definedName name="solver_rsd" localSheetId="3" hidden="1">0</definedName>
+    <definedName name="solver_scl" localSheetId="3" hidden="1">1</definedName>
+    <definedName name="solver_sho" localSheetId="3" hidden="1">2</definedName>
+    <definedName name="solver_ssz" localSheetId="3" hidden="1">100</definedName>
+    <definedName name="solver_tim" localSheetId="3" hidden="1">2147483647</definedName>
+    <definedName name="solver_tol" localSheetId="3" hidden="1">0.01</definedName>
+    <definedName name="solver_typ" localSheetId="3" hidden="1">3</definedName>
+    <definedName name="solver_val" localSheetId="3" hidden="1">0.000000000135</definedName>
+    <definedName name="solver_ver" localSheetId="3" hidden="1">3</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -4423,8 +4423,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:I33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -5254,7 +5254,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4C8F689-441D-42D9-88AF-5DCF32002981}">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
@@ -8609,6 +8609,321 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+  <dimension ref="A1:E29"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.44140625" style="62" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" style="62" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.109375" style="62" customWidth="1"/>
+    <col min="4" max="4" width="69.44140625" style="62" customWidth="1"/>
+    <col min="5" max="16384" width="11.44140625" style="62"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A1" s="76" t="s">
+        <v>92</v>
+      </c>
+      <c r="B1" s="217">
+        <v>10</v>
+      </c>
+      <c r="C1" s="91" t="s">
+        <v>93</v>
+      </c>
+      <c r="D1" s="218" t="s">
+        <v>163</v>
+      </c>
+      <c r="E1" s="69"/>
+    </row>
+    <row r="2" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="77" t="s">
+        <v>157</v>
+      </c>
+      <c r="B2" s="117" t="b">
+        <v>1</v>
+      </c>
+      <c r="C2" s="90" t="s">
+        <v>90</v>
+      </c>
+      <c r="D2" s="210" t="s">
+        <v>159</v>
+      </c>
+      <c r="E2" s="69"/>
+    </row>
+    <row r="3" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A3" s="77" t="s">
+        <v>160</v>
+      </c>
+      <c r="B3" s="116">
+        <f>(1/3)*10^(-3)</f>
+        <v>3.3333333333333332E-4</v>
+      </c>
+      <c r="C3" s="90" t="s">
+        <v>81</v>
+      </c>
+      <c r="D3" s="210" t="s">
+        <v>158</v>
+      </c>
+      <c r="E3" s="69"/>
+    </row>
+    <row r="4" spans="1:5" ht="43.2" x14ac:dyDescent="0.25">
+      <c r="A4" s="105" t="s">
+        <v>161</v>
+      </c>
+      <c r="B4" s="106" t="s">
+        <v>273</v>
+      </c>
+      <c r="C4" s="119" t="s">
+        <v>90</v>
+      </c>
+      <c r="D4" s="219" t="s">
+        <v>239</v>
+      </c>
+      <c r="E4" s="69"/>
+    </row>
+    <row r="5" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A5" s="77" t="s">
+        <v>39</v>
+      </c>
+      <c r="B5" s="98">
+        <v>20</v>
+      </c>
+      <c r="C5" s="90" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="210" t="s">
+        <v>162</v>
+      </c>
+      <c r="E5" s="69"/>
+    </row>
+    <row r="6" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A6" s="77" t="s">
+        <v>223</v>
+      </c>
+      <c r="B6" s="220">
+        <f>B5+273.15</f>
+        <v>293.14999999999998</v>
+      </c>
+      <c r="C6" s="90" t="s">
+        <v>41</v>
+      </c>
+      <c r="D6" s="210" t="s">
+        <v>222</v>
+      </c>
+      <c r="E6" s="69"/>
+    </row>
+    <row r="7" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A7" s="77" t="s">
+        <v>156</v>
+      </c>
+      <c r="B7" s="221">
+        <v>7</v>
+      </c>
+      <c r="C7" s="90" t="s">
+        <v>90</v>
+      </c>
+      <c r="D7" s="210" t="s">
+        <v>164</v>
+      </c>
+      <c r="E7" s="69"/>
+    </row>
+    <row r="8" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A8" s="77" t="s">
+        <v>155</v>
+      </c>
+      <c r="B8" s="222">
+        <f>B11/B12 * 4/3 * PI() *B10^3</f>
+        <v>1.3962634015954636E-10</v>
+      </c>
+      <c r="C8" s="90" t="s">
+        <v>91</v>
+      </c>
+      <c r="D8" s="210" t="s">
+        <v>251</v>
+      </c>
+      <c r="E8" s="69"/>
+    </row>
+    <row r="9" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A9" s="77" t="s">
+        <v>154</v>
+      </c>
+      <c r="B9" s="223">
+        <f>8.3144/1000</f>
+        <v>8.3143999999999996E-3</v>
+      </c>
+      <c r="C9" s="90" t="s">
+        <v>224</v>
+      </c>
+      <c r="D9" s="210" t="s">
+        <v>154</v>
+      </c>
+      <c r="E9" s="69"/>
+    </row>
+    <row r="10" spans="1:5" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A10" s="174" t="s">
+        <v>252</v>
+      </c>
+      <c r="B10" s="138">
+        <v>1E-4</v>
+      </c>
+      <c r="C10" s="90" t="s">
+        <v>87</v>
+      </c>
+      <c r="D10" s="224" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A11" s="77" t="s">
+        <v>254</v>
+      </c>
+      <c r="B11" s="225">
+        <v>100</v>
+      </c>
+      <c r="C11" s="90" t="s">
+        <v>255</v>
+      </c>
+      <c r="D11" s="226" t="s">
+        <v>256</v>
+      </c>
+      <c r="E11" s="69"/>
+    </row>
+    <row r="12" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="89" t="s">
+        <v>257</v>
+      </c>
+      <c r="B12" s="227">
+        <v>3</v>
+      </c>
+      <c r="C12" s="92" t="s">
+        <v>255</v>
+      </c>
+      <c r="D12" s="228" t="s">
+        <v>258</v>
+      </c>
+      <c r="E12" s="69"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13"/>
+      <c r="B13"/>
+      <c r="C13"/>
+      <c r="D13"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14"/>
+      <c r="B14"/>
+      <c r="C14"/>
+      <c r="D14"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15"/>
+      <c r="B15"/>
+      <c r="C15"/>
+      <c r="D15"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16"/>
+      <c r="B16"/>
+      <c r="C16"/>
+      <c r="D16"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17"/>
+      <c r="B17" s="189"/>
+      <c r="C17"/>
+      <c r="D17"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18"/>
+      <c r="B18"/>
+      <c r="C18"/>
+      <c r="D18"/>
+      <c r="E18" s="94"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B19"/>
+      <c r="C19"/>
+      <c r="D19"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B20"/>
+      <c r="C20"/>
+      <c r="D20"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B21"/>
+      <c r="C21"/>
+      <c r="D21"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B22"/>
+      <c r="C22"/>
+      <c r="D22"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B23"/>
+      <c r="C23"/>
+      <c r="D23"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B24"/>
+      <c r="C24"/>
+      <c r="D24"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B25"/>
+      <c r="C25"/>
+      <c r="D25"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B26"/>
+      <c r="C26"/>
+      <c r="D26"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="69"/>
+      <c r="B27"/>
+      <c r="C27"/>
+      <c r="D27"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B28"/>
+      <c r="C28"/>
+      <c r="D28"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B29"/>
+      <c r="C29"/>
+      <c r="D29"/>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="A1:D1">
+    <cfRule type="expression" dxfId="20" priority="1">
+      <formula>$B$2=TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A3:D4">
+    <cfRule type="expression" dxfId="19" priority="3">
+      <formula>$B$2 = FALSE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2" xr:uid="{28F6C65E-A04D-4413-835D-DA466EDD340E}">
+      <formula1>"TRUE, FALSE"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:E28"/>
   <sheetViews>
@@ -9077,321 +9392,6 @@
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:E29"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="21.44140625" style="62" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" style="62" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.109375" style="62" customWidth="1"/>
-    <col min="4" max="4" width="69.44140625" style="62" customWidth="1"/>
-    <col min="5" max="16384" width="11.44140625" style="62"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A1" s="76" t="s">
-        <v>92</v>
-      </c>
-      <c r="B1" s="217">
-        <v>10</v>
-      </c>
-      <c r="C1" s="91" t="s">
-        <v>93</v>
-      </c>
-      <c r="D1" s="218" t="s">
-        <v>163</v>
-      </c>
-      <c r="E1" s="69"/>
-    </row>
-    <row r="2" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A2" s="77" t="s">
-        <v>157</v>
-      </c>
-      <c r="B2" s="117" t="b">
-        <v>1</v>
-      </c>
-      <c r="C2" s="90" t="s">
-        <v>90</v>
-      </c>
-      <c r="D2" s="210" t="s">
-        <v>159</v>
-      </c>
-      <c r="E2" s="69"/>
-    </row>
-    <row r="3" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A3" s="77" t="s">
-        <v>160</v>
-      </c>
-      <c r="B3" s="116">
-        <f>(1/3)*10^(-3)</f>
-        <v>3.3333333333333332E-4</v>
-      </c>
-      <c r="C3" s="90" t="s">
-        <v>81</v>
-      </c>
-      <c r="D3" s="210" t="s">
-        <v>158</v>
-      </c>
-      <c r="E3" s="69"/>
-    </row>
-    <row r="4" spans="1:5" ht="43.2" x14ac:dyDescent="0.25">
-      <c r="A4" s="105" t="s">
-        <v>161</v>
-      </c>
-      <c r="B4" s="106" t="s">
-        <v>273</v>
-      </c>
-      <c r="C4" s="119" t="s">
-        <v>90</v>
-      </c>
-      <c r="D4" s="219" t="s">
-        <v>239</v>
-      </c>
-      <c r="E4" s="69"/>
-    </row>
-    <row r="5" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A5" s="77" t="s">
-        <v>39</v>
-      </c>
-      <c r="B5" s="98">
-        <v>20</v>
-      </c>
-      <c r="C5" s="90" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" s="210" t="s">
-        <v>162</v>
-      </c>
-      <c r="E5" s="69"/>
-    </row>
-    <row r="6" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A6" s="77" t="s">
-        <v>223</v>
-      </c>
-      <c r="B6" s="220">
-        <f>B5+273.15</f>
-        <v>293.14999999999998</v>
-      </c>
-      <c r="C6" s="90" t="s">
-        <v>41</v>
-      </c>
-      <c r="D6" s="210" t="s">
-        <v>222</v>
-      </c>
-      <c r="E6" s="69"/>
-    </row>
-    <row r="7" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A7" s="77" t="s">
-        <v>156</v>
-      </c>
-      <c r="B7" s="221">
-        <v>7</v>
-      </c>
-      <c r="C7" s="90" t="s">
-        <v>90</v>
-      </c>
-      <c r="D7" s="210" t="s">
-        <v>164</v>
-      </c>
-      <c r="E7" s="69"/>
-    </row>
-    <row r="8" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A8" s="77" t="s">
-        <v>155</v>
-      </c>
-      <c r="B8" s="222">
-        <f>B11/B12 * 4/3 * PI() *B10^3</f>
-        <v>1.3962634015954636E-10</v>
-      </c>
-      <c r="C8" s="90" t="s">
-        <v>91</v>
-      </c>
-      <c r="D8" s="210" t="s">
-        <v>251</v>
-      </c>
-      <c r="E8" s="69"/>
-    </row>
-    <row r="9" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A9" s="77" t="s">
-        <v>154</v>
-      </c>
-      <c r="B9" s="223">
-        <f>8.3144/1000</f>
-        <v>8.3143999999999996E-3</v>
-      </c>
-      <c r="C9" s="90" t="s">
-        <v>224</v>
-      </c>
-      <c r="D9" s="210" t="s">
-        <v>154</v>
-      </c>
-      <c r="E9" s="69"/>
-    </row>
-    <row r="10" spans="1:5" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A10" s="174" t="s">
-        <v>252</v>
-      </c>
-      <c r="B10" s="138">
-        <v>1E-4</v>
-      </c>
-      <c r="C10" s="90" t="s">
-        <v>87</v>
-      </c>
-      <c r="D10" s="224" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A11" s="77" t="s">
-        <v>254</v>
-      </c>
-      <c r="B11" s="225">
-        <v>100</v>
-      </c>
-      <c r="C11" s="90" t="s">
-        <v>255</v>
-      </c>
-      <c r="D11" s="226" t="s">
-        <v>256</v>
-      </c>
-      <c r="E11" s="69"/>
-    </row>
-    <row r="12" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="89" t="s">
-        <v>257</v>
-      </c>
-      <c r="B12" s="227">
-        <v>3</v>
-      </c>
-      <c r="C12" s="92" t="s">
-        <v>255</v>
-      </c>
-      <c r="D12" s="228" t="s">
-        <v>258</v>
-      </c>
-      <c r="E12" s="69"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13"/>
-      <c r="B13"/>
-      <c r="C13"/>
-      <c r="D13"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14"/>
-      <c r="B14"/>
-      <c r="C14"/>
-      <c r="D14"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15"/>
-      <c r="B15"/>
-      <c r="C15"/>
-      <c r="D15"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16"/>
-      <c r="B16"/>
-      <c r="C16"/>
-      <c r="D16"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17"/>
-      <c r="B17" s="189"/>
-      <c r="C17"/>
-      <c r="D17"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18"/>
-      <c r="B18"/>
-      <c r="C18"/>
-      <c r="D18"/>
-      <c r="E18" s="94"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B19"/>
-      <c r="C19"/>
-      <c r="D19"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B20"/>
-      <c r="C20"/>
-      <c r="D20"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B21"/>
-      <c r="C21"/>
-      <c r="D21"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B22"/>
-      <c r="C22"/>
-      <c r="D22"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B23"/>
-      <c r="C23"/>
-      <c r="D23"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B24"/>
-      <c r="C24"/>
-      <c r="D24"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B25"/>
-      <c r="C25"/>
-      <c r="D25"/>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B26"/>
-      <c r="C26"/>
-      <c r="D26"/>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="69"/>
-      <c r="B27"/>
-      <c r="C27"/>
-      <c r="D27"/>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B28"/>
-      <c r="C28"/>
-      <c r="D28"/>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B29"/>
-      <c r="C29"/>
-      <c r="D29"/>
-    </row>
-  </sheetData>
-  <conditionalFormatting sqref="A1:D1">
-    <cfRule type="expression" dxfId="20" priority="1">
-      <formula>$B$2=TRUE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A3:D4">
-    <cfRule type="expression" dxfId="19" priority="3">
-      <formula>$B$2 = FALSE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2" xr:uid="{28F6C65E-A04D-4413-835D-DA466EDD340E}">
-      <formula1>"TRUE, FALSE"</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -10073,7 +10073,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:J14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Extracting Ks and Ki
Implemented the extraction of Ks and Ki from the excel and stored them in the struct constants. Also did some extra commenting.
</commit_message>
<xml_diff>
--- a/lib/pre-processing/test_file.xlsx
+++ b/lib/pre-processing/test_file.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tsbie\Documents\Universiteit\Master\Jaar 2\MEP\Code\IbM-Fermentation\IbM-Fermentation\lib\pre-processing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{691D60B8-FDC5-49F6-87B5-71A8A05F3C8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB980C5E-64B0-4AAE-9273-4D26932827AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14310" yWindow="-16200" windowWidth="14610" windowHeight="15585" tabRatio="808" firstSheet="5" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14310" yWindow="-16200" windowWidth="14610" windowHeight="15585" tabRatio="808" firstSheet="8" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Information" sheetId="30" r:id="rId1"/>
@@ -3578,6 +3578,9 @@
     <xf numFmtId="0" fontId="36" fillId="0" borderId="22" xfId="10" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="10" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="25" fillId="10" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3588,9 +3591,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="10" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="10" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3620,13 +3620,6 @@
     <dxf>
       <font>
         <color theme="0" tint="-0.34998626667073579"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-        <color theme="1" tint="0.34998626667073579"/>
       </font>
     </dxf>
     <dxf>
@@ -3701,23 +3694,10 @@
     </dxf>
     <dxf>
       <font>
-        <color theme="0" tint="-0.24994659260841701"/>
+        <b val="0"/>
+        <i/>
+        <color theme="1" tint="0.34998626667073579"/>
       </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.24994659260841701"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <font>
@@ -3792,6 +3772,26 @@
     <dxf>
       <font>
         <strike val="0"/>
+        <color theme="0" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color theme="0" tint="-0.24994659260841701"/>
       </font>
       <fill>
@@ -4423,8 +4423,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:I33"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -4770,7 +4770,7 @@
         <v>0</v>
       </c>
       <c r="H13" s="72"/>
-      <c r="I13" s="274" t="s">
+      <c r="I13" s="275" t="s">
         <v>229</v>
       </c>
     </row>
@@ -4795,7 +4795,7 @@
         <v>0</v>
       </c>
       <c r="H14" s="72"/>
-      <c r="I14" s="274"/>
+      <c r="I14" s="275"/>
     </row>
     <row r="15" spans="1:9" s="71" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A15" s="77" t="s">
@@ -4818,7 +4818,7 @@
         <v>0</v>
       </c>
       <c r="H15" s="72"/>
-      <c r="I15" s="274"/>
+      <c r="I15" s="275"/>
     </row>
     <row r="16" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A16" s="77" t="s">
@@ -4841,7 +4841,7 @@
         <v>0</v>
       </c>
       <c r="F16" s="71"/>
-      <c r="I16" s="274"/>
+      <c r="I16" s="275"/>
     </row>
     <row r="17" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A17" s="77" t="s">
@@ -4863,7 +4863,7 @@
         <v>0</v>
       </c>
       <c r="F17" s="71"/>
-      <c r="I17" s="274"/>
+      <c r="I17" s="275"/>
     </row>
     <row r="18" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A18" s="127" t="s">
@@ -4886,7 +4886,7 @@
         <v>0</v>
       </c>
       <c r="F18" s="71"/>
-      <c r="I18" s="274"/>
+      <c r="I18" s="275"/>
     </row>
     <row r="19" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A19" s="77" t="s">
@@ -4908,7 +4908,7 @@
         <v>0</v>
       </c>
       <c r="F19" s="71"/>
-      <c r="I19" s="274"/>
+      <c r="I19" s="275"/>
     </row>
     <row r="20" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A20" s="133" t="s">
@@ -4931,7 +4931,7 @@
         <v>0</v>
       </c>
       <c r="F20" s="71"/>
-      <c r="I20" s="274"/>
+      <c r="I20" s="275"/>
     </row>
     <row r="21" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A21" s="139" t="s">
@@ -4955,7 +4955,7 @@
       </c>
       <c r="F21" s="71"/>
       <c r="H21" s="71"/>
-      <c r="I21" s="274"/>
+      <c r="I21" s="275"/>
     </row>
     <row r="22" spans="1:9" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="140" t="s">
@@ -4978,17 +4978,17 @@
         <v>0</v>
       </c>
       <c r="F22" s="71"/>
-      <c r="I22" s="274"/>
+      <c r="I22" s="275"/>
     </row>
     <row r="23" spans="1:9" ht="28.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="271" t="s">
+      <c r="A23" s="272" t="s">
         <v>217</v>
       </c>
-      <c r="B23" s="272"/>
-      <c r="C23" s="272"/>
-      <c r="D23" s="272"/>
-      <c r="E23" s="272"/>
-      <c r="F23" s="273"/>
+      <c r="B23" s="273"/>
+      <c r="C23" s="273"/>
+      <c r="D23" s="273"/>
+      <c r="E23" s="273"/>
+      <c r="F23" s="274"/>
     </row>
     <row r="24" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A24" s="76" t="s">
@@ -5009,7 +5009,7 @@
       <c r="F24" s="152" t="s">
         <v>86</v>
       </c>
-      <c r="I24" s="274" t="s">
+      <c r="I24" s="275" t="s">
         <v>230</v>
       </c>
     </row>
@@ -5032,7 +5032,7 @@
       <c r="F25" s="152" t="s">
         <v>86</v>
       </c>
-      <c r="I25" s="274"/>
+      <c r="I25" s="275"/>
     </row>
     <row r="26" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A26" s="77" t="s">
@@ -5053,7 +5053,7 @@
       <c r="F26" s="152" t="s">
         <v>86</v>
       </c>
-      <c r="I26" s="274"/>
+      <c r="I26" s="275"/>
     </row>
     <row r="27" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A27" s="77" t="s">
@@ -5074,7 +5074,7 @@
       <c r="F27" s="152" t="s">
         <v>86</v>
       </c>
-      <c r="I27" s="274"/>
+      <c r="I27" s="275"/>
     </row>
     <row r="28" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A28" s="77" t="s">
@@ -5095,7 +5095,7 @@
       <c r="F28" s="204" t="s">
         <v>86</v>
       </c>
-      <c r="I28" s="274"/>
+      <c r="I28" s="275"/>
     </row>
     <row r="29" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A29" s="127" t="s">
@@ -5116,7 +5116,7 @@
       <c r="F29" s="205" t="s">
         <v>86</v>
       </c>
-      <c r="I29" s="274"/>
+      <c r="I29" s="275"/>
     </row>
     <row r="30" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A30" s="77" t="s">
@@ -5137,7 +5137,7 @@
       <c r="F30" s="204" t="s">
         <v>86</v>
       </c>
-      <c r="I30" s="274"/>
+      <c r="I30" s="275"/>
     </row>
     <row r="31" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A31" s="133" t="s">
@@ -5158,7 +5158,7 @@
       <c r="F31" s="155" t="s">
         <v>86</v>
       </c>
-      <c r="I31" s="274"/>
+      <c r="I31" s="275"/>
     </row>
     <row r="32" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A32" s="139" t="s">
@@ -5179,7 +5179,7 @@
       <c r="F32" s="205" t="s">
         <v>86</v>
       </c>
-      <c r="I32" s="274"/>
+      <c r="I32" s="275"/>
     </row>
     <row r="33" spans="1:9" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="140" t="s">
@@ -5200,7 +5200,7 @@
       <c r="F33" s="152" t="s">
         <v>86</v>
       </c>
-      <c r="I33" s="274"/>
+      <c r="I33" s="275"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -5210,37 +5210,37 @@
     <mergeCell ref="I24:I33"/>
   </mergeCells>
   <conditionalFormatting sqref="B18:B22 D19">
-    <cfRule type="cellIs" dxfId="11" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="4" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="5" operator="containsText" text="NA">
+    <cfRule type="containsText" dxfId="9" priority="5" operator="containsText" text="NA">
       <formula>NOT(ISERROR(SEARCH("NA",B18)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="9" priority="6" operator="containsText" text="Inf">
+    <cfRule type="containsText" dxfId="8" priority="6" operator="containsText" text="Inf">
       <formula>NOT(ISERROR(SEARCH("Inf",B18)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13:E17 C18:D18 E18:E22">
-    <cfRule type="cellIs" dxfId="8" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="7" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:F11 B13:E17 C18:D18 E18:E22 B24:F33">
-    <cfRule type="containsText" dxfId="7" priority="60" operator="containsText" text="NA">
+    <cfRule type="containsText" dxfId="6" priority="60" operator="containsText" text="NA">
       <formula>NOT(ISERROR(SEARCH("NA",B2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="61" operator="containsText" text="Inf">
+    <cfRule type="containsText" dxfId="5" priority="61" operator="containsText" text="Inf">
       <formula>NOT(ISERROR(SEARCH("Inf",B2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C20:D22">
-    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="NA">
+    <cfRule type="containsText" dxfId="3" priority="2" operator="containsText" text="NA">
       <formula>NOT(ISERROR(SEARCH("NA",C20)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="Inf">
+    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="Inf">
       <formula>NOT(ISERROR(SEARCH("Inf",C20)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5255,7 +5255,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -5280,7 +5280,7 @@
       <c r="E1" s="136" t="s">
         <v>76</v>
       </c>
-      <c r="F1" s="275" t="s">
+      <c r="F1" s="271" t="s">
         <v>277</v>
       </c>
     </row>
@@ -5300,7 +5300,7 @@
       <c r="E2" s="100">
         <v>0</v>
       </c>
-      <c r="F2" s="275"/>
+      <c r="F2" s="271"/>
     </row>
     <row r="3" spans="1:6" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="77" t="s">
@@ -5318,7 +5318,7 @@
       <c r="E3" s="100">
         <v>0</v>
       </c>
-      <c r="F3" s="275"/>
+      <c r="F3" s="271"/>
     </row>
     <row r="4" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="89" t="s">
@@ -5336,7 +5336,7 @@
       <c r="E4" s="100">
         <v>0</v>
       </c>
-      <c r="F4" s="275"/>
+      <c r="F4" s="271"/>
     </row>
     <row r="5" spans="1:6" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F5" s="173"/>
@@ -5350,7 +5350,7 @@
   </mergeCells>
   <phoneticPr fontId="38" type="noConversion"/>
   <conditionalFormatting sqref="B2:E6">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5363,7 +5363,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -5384,7 +5384,7 @@
       <c r="D1" s="136" t="s">
         <v>17</v>
       </c>
-      <c r="E1" s="275" t="s">
+      <c r="E1" s="271" t="s">
         <v>276</v>
       </c>
     </row>
@@ -5401,7 +5401,7 @@
       <c r="D2" s="100">
         <v>0</v>
       </c>
-      <c r="E2" s="275"/>
+      <c r="E2" s="271"/>
     </row>
     <row r="3" spans="1:5" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="77" t="s">
@@ -5416,7 +5416,7 @@
       <c r="D3" s="100">
         <v>0</v>
       </c>
-      <c r="E3" s="275"/>
+      <c r="E3" s="271"/>
     </row>
     <row r="4" spans="1:5" ht="13.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="89" t="s">
@@ -5431,7 +5431,7 @@
       <c r="D4" s="100">
         <v>0</v>
       </c>
-      <c r="E4" s="275"/>
+      <c r="E4" s="271"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -8903,12 +8903,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:D1">
-    <cfRule type="expression" dxfId="20" priority="1">
+    <cfRule type="expression" dxfId="21" priority="1">
       <formula>$B$2=TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3:D4">
-    <cfRule type="expression" dxfId="19" priority="3">
+    <cfRule type="expression" dxfId="20" priority="3">
       <formula>$B$2 = FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9381,7 +9381,7 @@
     <mergeCell ref="E15:E28"/>
   </mergeCells>
   <conditionalFormatting sqref="A16:D28">
-    <cfRule type="expression" dxfId="21" priority="1">
+    <cfRule type="expression" dxfId="19" priority="1">
       <formula>$B$15 = FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9563,7 +9563,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A8" workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
@@ -10073,7 +10073,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:J14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
First complete draft loadPresetFile
Changed variable names to something more specific. Also, added collect(skipmissing()) at some places. Currently not required but just in case for the future
</commit_message>
<xml_diff>
--- a/lib/pre-processing/test_file.xlsx
+++ b/lib/pre-processing/test_file.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tsbie\Documents\Universiteit\Master\Jaar 2\MEP\Code\IbM-Fermentation\IbM-Fermentation\lib\pre-processing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB980C5E-64B0-4AAE-9273-4D26932827AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82AAD9FD-0CCB-4C47-81E9-B4C303FF0A10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14310" yWindow="-16200" windowWidth="14610" windowHeight="15585" tabRatio="808" firstSheet="8" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14310" yWindow="-16200" windowWidth="14610" windowHeight="15585" tabRatio="808" firstSheet="3" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Information" sheetId="30" r:id="rId1"/>
@@ -3578,9 +3578,6 @@
     <xf numFmtId="0" fontId="36" fillId="0" borderId="22" xfId="10" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="10" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="25" fillId="10" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3591,6 +3588,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="10" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="10" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3620,6 +3620,13 @@
     <dxf>
       <font>
         <color theme="0" tint="-0.34998626667073579"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <color theme="1" tint="0.34998626667073579"/>
       </font>
     </dxf>
     <dxf>
@@ -3690,13 +3697,6 @@
         <b val="0"/>
         <i/>
         <color theme="0" tint="-0.34998626667073579"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-        <color theme="1" tint="0.34998626667073579"/>
       </font>
     </dxf>
     <dxf>
@@ -4423,8 +4423,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:I33"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -4770,7 +4770,7 @@
         <v>0</v>
       </c>
       <c r="H13" s="72"/>
-      <c r="I13" s="275" t="s">
+      <c r="I13" s="274" t="s">
         <v>229</v>
       </c>
     </row>
@@ -4795,7 +4795,7 @@
         <v>0</v>
       </c>
       <c r="H14" s="72"/>
-      <c r="I14" s="275"/>
+      <c r="I14" s="274"/>
     </row>
     <row r="15" spans="1:9" s="71" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A15" s="77" t="s">
@@ -4818,7 +4818,7 @@
         <v>0</v>
       </c>
       <c r="H15" s="72"/>
-      <c r="I15" s="275"/>
+      <c r="I15" s="274"/>
     </row>
     <row r="16" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A16" s="77" t="s">
@@ -4841,7 +4841,7 @@
         <v>0</v>
       </c>
       <c r="F16" s="71"/>
-      <c r="I16" s="275"/>
+      <c r="I16" s="274"/>
     </row>
     <row r="17" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A17" s="77" t="s">
@@ -4863,7 +4863,7 @@
         <v>0</v>
       </c>
       <c r="F17" s="71"/>
-      <c r="I17" s="275"/>
+      <c r="I17" s="274"/>
     </row>
     <row r="18" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A18" s="127" t="s">
@@ -4886,7 +4886,7 @@
         <v>0</v>
       </c>
       <c r="F18" s="71"/>
-      <c r="I18" s="275"/>
+      <c r="I18" s="274"/>
     </row>
     <row r="19" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A19" s="77" t="s">
@@ -4908,7 +4908,7 @@
         <v>0</v>
       </c>
       <c r="F19" s="71"/>
-      <c r="I19" s="275"/>
+      <c r="I19" s="274"/>
     </row>
     <row r="20" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A20" s="133" t="s">
@@ -4931,7 +4931,7 @@
         <v>0</v>
       </c>
       <c r="F20" s="71"/>
-      <c r="I20" s="275"/>
+      <c r="I20" s="274"/>
     </row>
     <row r="21" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A21" s="139" t="s">
@@ -4955,7 +4955,7 @@
       </c>
       <c r="F21" s="71"/>
       <c r="H21" s="71"/>
-      <c r="I21" s="275"/>
+      <c r="I21" s="274"/>
     </row>
     <row r="22" spans="1:9" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="140" t="s">
@@ -4978,17 +4978,17 @@
         <v>0</v>
       </c>
       <c r="F22" s="71"/>
-      <c r="I22" s="275"/>
+      <c r="I22" s="274"/>
     </row>
     <row r="23" spans="1:9" ht="28.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="272" t="s">
+      <c r="A23" s="271" t="s">
         <v>217</v>
       </c>
-      <c r="B23" s="273"/>
-      <c r="C23" s="273"/>
-      <c r="D23" s="273"/>
-      <c r="E23" s="273"/>
-      <c r="F23" s="274"/>
+      <c r="B23" s="272"/>
+      <c r="C23" s="272"/>
+      <c r="D23" s="272"/>
+      <c r="E23" s="272"/>
+      <c r="F23" s="273"/>
     </row>
     <row r="24" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A24" s="76" t="s">
@@ -5009,7 +5009,7 @@
       <c r="F24" s="152" t="s">
         <v>86</v>
       </c>
-      <c r="I24" s="275" t="s">
+      <c r="I24" s="274" t="s">
         <v>230</v>
       </c>
     </row>
@@ -5032,7 +5032,7 @@
       <c r="F25" s="152" t="s">
         <v>86</v>
       </c>
-      <c r="I25" s="275"/>
+      <c r="I25" s="274"/>
     </row>
     <row r="26" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A26" s="77" t="s">
@@ -5053,7 +5053,7 @@
       <c r="F26" s="152" t="s">
         <v>86</v>
       </c>
-      <c r="I26" s="275"/>
+      <c r="I26" s="274"/>
     </row>
     <row r="27" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A27" s="77" t="s">
@@ -5074,7 +5074,7 @@
       <c r="F27" s="152" t="s">
         <v>86</v>
       </c>
-      <c r="I27" s="275"/>
+      <c r="I27" s="274"/>
     </row>
     <row r="28" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A28" s="77" t="s">
@@ -5095,7 +5095,7 @@
       <c r="F28" s="204" t="s">
         <v>86</v>
       </c>
-      <c r="I28" s="275"/>
+      <c r="I28" s="274"/>
     </row>
     <row r="29" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A29" s="127" t="s">
@@ -5116,7 +5116,7 @@
       <c r="F29" s="205" t="s">
         <v>86</v>
       </c>
-      <c r="I29" s="275"/>
+      <c r="I29" s="274"/>
     </row>
     <row r="30" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A30" s="77" t="s">
@@ -5137,7 +5137,7 @@
       <c r="F30" s="204" t="s">
         <v>86</v>
       </c>
-      <c r="I30" s="275"/>
+      <c r="I30" s="274"/>
     </row>
     <row r="31" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A31" s="133" t="s">
@@ -5158,7 +5158,7 @@
       <c r="F31" s="155" t="s">
         <v>86</v>
       </c>
-      <c r="I31" s="275"/>
+      <c r="I31" s="274"/>
     </row>
     <row r="32" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A32" s="139" t="s">
@@ -5179,7 +5179,7 @@
       <c r="F32" s="205" t="s">
         <v>86</v>
       </c>
-      <c r="I32" s="275"/>
+      <c r="I32" s="274"/>
     </row>
     <row r="33" spans="1:9" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="140" t="s">
@@ -5200,7 +5200,7 @@
       <c r="F33" s="152" t="s">
         <v>86</v>
       </c>
-      <c r="I33" s="275"/>
+      <c r="I33" s="274"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -5210,37 +5210,37 @@
     <mergeCell ref="I24:I33"/>
   </mergeCells>
   <conditionalFormatting sqref="B18:B22 D19">
-    <cfRule type="cellIs" dxfId="10" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="4" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="9" priority="5" operator="containsText" text="NA">
+    <cfRule type="containsText" dxfId="10" priority="5" operator="containsText" text="NA">
       <formula>NOT(ISERROR(SEARCH("NA",B18)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="6" operator="containsText" text="Inf">
+    <cfRule type="containsText" dxfId="9" priority="6" operator="containsText" text="Inf">
       <formula>NOT(ISERROR(SEARCH("Inf",B18)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13:E17 C18:D18 E18:E22">
-    <cfRule type="cellIs" dxfId="7" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="7" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:F11 B13:E17 C18:D18 E18:E22 B24:F33">
-    <cfRule type="containsText" dxfId="6" priority="60" operator="containsText" text="NA">
+    <cfRule type="containsText" dxfId="7" priority="60" operator="containsText" text="NA">
       <formula>NOT(ISERROR(SEARCH("NA",B2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="5" priority="61" operator="containsText" text="Inf">
+    <cfRule type="containsText" dxfId="6" priority="61" operator="containsText" text="Inf">
       <formula>NOT(ISERROR(SEARCH("Inf",B2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C20:D22">
-    <cfRule type="cellIs" dxfId="4" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="2" operator="containsText" text="NA">
+    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="NA">
       <formula>NOT(ISERROR(SEARCH("NA",C20)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="Inf">
+    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="Inf">
       <formula>NOT(ISERROR(SEARCH("Inf",C20)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5254,7 +5254,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4C8F689-441D-42D9-88AF-5DCF32002981}">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
@@ -5280,7 +5280,7 @@
       <c r="E1" s="136" t="s">
         <v>76</v>
       </c>
-      <c r="F1" s="271" t="s">
+      <c r="F1" s="275" t="s">
         <v>277</v>
       </c>
     </row>
@@ -5300,7 +5300,7 @@
       <c r="E2" s="100">
         <v>0</v>
       </c>
-      <c r="F2" s="271"/>
+      <c r="F2" s="275"/>
     </row>
     <row r="3" spans="1:6" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="77" t="s">
@@ -5318,7 +5318,7 @@
       <c r="E3" s="100">
         <v>0</v>
       </c>
-      <c r="F3" s="271"/>
+      <c r="F3" s="275"/>
     </row>
     <row r="4" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="89" t="s">
@@ -5336,7 +5336,7 @@
       <c r="E4" s="100">
         <v>0</v>
       </c>
-      <c r="F4" s="271"/>
+      <c r="F4" s="275"/>
     </row>
     <row r="5" spans="1:6" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F5" s="173"/>
@@ -5350,7 +5350,7 @@
   </mergeCells>
   <phoneticPr fontId="38" type="noConversion"/>
   <conditionalFormatting sqref="B2:E6">
-    <cfRule type="cellIs" dxfId="11" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5384,7 +5384,7 @@
       <c r="D1" s="136" t="s">
         <v>17</v>
       </c>
-      <c r="E1" s="271" t="s">
+      <c r="E1" s="275" t="s">
         <v>276</v>
       </c>
     </row>
@@ -5401,7 +5401,7 @@
       <c r="D2" s="100">
         <v>0</v>
       </c>
-      <c r="E2" s="271"/>
+      <c r="E2" s="275"/>
     </row>
     <row r="3" spans="1:5" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="77" t="s">
@@ -5416,7 +5416,7 @@
       <c r="D3" s="100">
         <v>0</v>
       </c>
-      <c r="E3" s="271"/>
+      <c r="E3" s="275"/>
     </row>
     <row r="4" spans="1:5" ht="13.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="89" t="s">
@@ -5431,7 +5431,7 @@
       <c r="D4" s="100">
         <v>0</v>
       </c>
-      <c r="E4" s="271"/>
+      <c r="E4" s="275"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -5451,7 +5451,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -5557,7 +5557,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="M14" sqref="M14"/>
+      <selection pane="bottomRight" activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -8927,7 +8927,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
@@ -9563,8 +9563,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -10073,8 +10073,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:J14"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1:E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>

</xml_diff>